<commit_message>
Article: Lembar Kerja: Number Format
</commit_message>
<xml_diff>
--- a/assets/posts/lembarkerja/2018/06/01-number.xlsx
+++ b/assets/posts/lembarkerja/2018/06/01-number.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Angka" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Tanggal" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Pajak" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Rupiah" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Unit" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="67">
   <si>
     <t xml:space="preserve">Format</t>
   </si>
@@ -200,13 +201,37 @@
   </si>
   <si>
     <t xml:space="preserve">" Rp"* -# ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nilai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[=0]-;0,00" kg"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[&gt;=1000000]0,00.." ton";[&gt;=1000]0,00."  kg";0" gram"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[HH]:MM:SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waktu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[=0]-;[&gt;=20]#.###" km/h";#.##0,00" km/h"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kecepatan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="30">
+  <numFmts count="35">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="00"/>
@@ -237,6 +262,11 @@
     <numFmt numFmtId="191" formatCode="* #,##0.00\ ;* \(#,##0.00\);* \-#\ ;[RED]&quot;Nilai &quot;@\?"/>
     <numFmt numFmtId="192" formatCode="&quot; Rp&quot;* #,##0.00\ ;&quot;-Rp&quot;* #,##0.00\ ;&quot; Rp&quot;* \-#\ ;@\ "/>
     <numFmt numFmtId="193" formatCode="&quot; Rp&quot;* #,##0.00\ ;&quot;-Rp&quot;* #,##0.00\ ;&quot; Rp&quot;* \-#\ ;@"/>
+    <numFmt numFmtId="194" formatCode="[=0]\-;0.00&quot; m&quot;"/>
+    <numFmt numFmtId="195" formatCode="[=0]\-;0.00&quot; kg&quot;"/>
+    <numFmt numFmtId="196" formatCode="[&gt;=1000000]0.00,,&quot; ton&quot;;[&gt;=1000]0.00,&quot; kg&quot;;0&quot; gram&quot;"/>
+    <numFmt numFmtId="197" formatCode="[hh]:mm:ss"/>
+    <numFmt numFmtId="198" formatCode="[=0]\-;[&gt;=20]#,###&quot; km/h&quot;;#,##0.00&quot; km/h&quot;"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -457,7 +487,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="72">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -696,6 +726,54 @@
     </xf>
     <xf numFmtId="193" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="194" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="195" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="196" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="197" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="198" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -757,7 +835,7 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF004D40"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -778,8 +856,8 @@
   </sheetPr>
   <dimension ref="B1:C23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -925,7 +1003,7 @@
   <dimension ref="B1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1208,7 +1286,7 @@
   </sheetPr>
   <dimension ref="B1:G38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -1644,4 +1722,332 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF004D40"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:D34"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="60" width="20.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="22" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="2.55"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="4"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="63"/>
+      <c r="D4" s="64"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="66"/>
+      <c r="D5" s="67"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="61" t="n">
+        <v>0.1892</v>
+      </c>
+      <c r="D6" s="68" t="n">
+        <v>0.1892</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="61" t="n">
+        <v>182.3268</v>
+      </c>
+      <c r="D8" s="68" t="n">
+        <v>182.3268</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="4"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="23"/>
+    </row>
+    <row r="10" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="4"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="23"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="66"/>
+      <c r="D12" s="67"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="61" t="n">
+        <v>24</v>
+      </c>
+      <c r="D13" s="69" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="61" t="n">
+        <v>256</v>
+      </c>
+      <c r="D14" s="69" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="61" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D15" s="69" t="n">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="61" t="n">
+        <v>65536</v>
+      </c>
+      <c r="D16" s="69" t="n">
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="61" t="n">
+        <v>2777216</v>
+      </c>
+      <c r="D17" s="69" t="n">
+        <v>2777216</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="4"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="23"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="63"/>
+      <c r="D19" s="64"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="66"/>
+      <c r="D20" s="67"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="61" t="n">
+        <v>0.000254629601840861</v>
+      </c>
+      <c r="D21" s="70" t="n">
+        <v>0.000254629601840861</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="61" t="n">
+        <v>0.00035879630013369</v>
+      </c>
+      <c r="D22" s="70" t="n">
+        <v>0.00035879630013369</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="61" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D23" s="70" t="n">
+        <v>0.004</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="4"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="23"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="63"/>
+      <c r="D26" s="64"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="66"/>
+      <c r="D27" s="67"/>
+    </row>
+    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="61" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D28" s="71" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="D29" s="71" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="61" t="n">
+        <v>24</v>
+      </c>
+      <c r="D30" s="71" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="61" t="n">
+        <v>256</v>
+      </c>
+      <c r="D31" s="71" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="61" t="n">
+        <v>4096</v>
+      </c>
+      <c r="D32" s="71" t="n">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="61" t="n">
+        <v>65536</v>
+      </c>
+      <c r="D33" s="71" t="n">
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="4"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="23"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Article: Lembar Kerja: Contoh Kasus
</commit_message>
<xml_diff>
--- a/assets/posts/lembarkerja/2018/06/01-number.xlsx
+++ b/assets/posts/lembarkerja/2018/06/01-number.xlsx
@@ -14,6 +14,9 @@
     <sheet name="Rupiah" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Unit" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">Unit!$A$1:$E$35</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -1732,8 +1735,8 @@
   </sheetPr>
   <dimension ref="B1:D34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>